<commit_message>
save as EXCEL done
</commit_message>
<xml_diff>
--- a/database.XLSX
+++ b/database.XLSX
@@ -2,13 +2,17 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
+  <workbookPr defaultThemeVersion="164011"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Studying\Coursework\proj\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="10632" windowHeight="11172"/>
   </bookViews>
   <sheets>
-    <sheet name="Rock" sheetId="3" r:id="rId1"/>
-    <sheet name="Pop" sheetId="2" r:id="rId2"/>
+    <sheet name="Rock" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -20,98 +24,49 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+  <si>
+    <t>№</t>
+  </si>
   <si>
     <t>Song</t>
   </si>
   <si>
-    <t>Singer</t>
+    <t>Artist</t>
+  </si>
+  <si>
+    <t>Views</t>
   </si>
   <si>
     <t>Beggin</t>
   </si>
   <si>
+    <t>Maneskin</t>
+  </si>
+  <si>
     <t>Careless Whisper</t>
   </si>
   <si>
-    <t>I WANNA BE YOUR SLAVE</t>
-  </si>
-  <si>
     <t>George Michael</t>
   </si>
   <si>
-    <t>Cold Heart (PNAU Remix)</t>
-  </si>
-  <si>
-    <t>Elton John &amp; Dua Lipa</t>
-  </si>
-  <si>
-    <t>Easy On Me</t>
-  </si>
-  <si>
-    <t>Adele</t>
-  </si>
-  <si>
-    <t>Stay</t>
-  </si>
-  <si>
-    <t>The Kid LAROI &amp; Justin Bieber</t>
-  </si>
-  <si>
-    <t>Maneskin</t>
-  </si>
-  <si>
-    <t>№</t>
+    <t>Notion</t>
+  </si>
+  <si>
+    <t>unknown</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="6" x14ac:knownFonts="1">
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="204"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <charset val="204"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <charset val="204"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color theme="10"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <name val="Calibri"/>
-      <family val="2"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -132,21 +87,13 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="2">
-    <cellStyle name="Гиперссылка" xfId="1" builtinId="8"/>
+  <cellStyles count="1">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -425,136 +372,71 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C4"/>
+  <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="A2" sqref="A2:D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="1" max="1" width="9" customWidth="1"/>
-    <col min="2" max="2" width="29.44140625" customWidth="1"/>
-    <col min="3" max="3" width="27" customWidth="1"/>
-  </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A1" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="B1" s="1" t="s">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="B1" t="s">
         <v>1</v>
       </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>1</v>
       </c>
-      <c r="B2" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="C2" s="3" t="s">
-        <v>12</v>
+      <c r="B2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D2">
+        <v>142544584</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>2</v>
       </c>
-      <c r="B3" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="C3" s="3" t="s">
-        <v>5</v>
+      <c r="B3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D3">
+        <v>802156270</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>3</v>
       </c>
-      <c r="B4" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="C4" s="3" t="s">
-        <v>12</v>
+      <c r="B4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C4" t="s">
+        <v>9</v>
+      </c>
+      <c r="D4">
+        <v>5888851</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C4"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="2" max="2" width="26.44140625" customWidth="1"/>
-    <col min="3" max="3" width="27.21875" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A1" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A2">
-        <v>1</v>
-      </c>
-      <c r="B2" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="C2" s="4" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A3">
-        <v>2</v>
-      </c>
-      <c r="B3" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="C3" s="4" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A4">
-        <v>3</v>
-      </c>
-      <c r="B4" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="C4" s="4" t="s">
-        <v>11</v>
-      </c>
-    </row>
-  </sheetData>
-  <hyperlinks>
-    <hyperlink ref="B2" r:id="rId1" display="https://www.shazam.com/track/579595745/cold-heart-pnau-remix"/>
-    <hyperlink ref="C2" r:id="rId2" display="https://www.shazam.com/artist/3647/elton-john"/>
-    <hyperlink ref="B3" r:id="rId3" display="https://www.shazam.com/track/587472945/easy-on-me"/>
-    <hyperlink ref="C3" r:id="rId4" display="https://www.shazam.com/artist/10080114/adele"/>
-    <hyperlink ref="B4" r:id="rId5" display="https://www.shazam.com/track/552221348/stay"/>
-    <hyperlink ref="C4" r:id="rId6" display="https://www.shazam.com/artist/205204904/the-kid-laroi"/>
-  </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId7"/>
-</worksheet>
 </file>
</xml_diff>